<commit_message>
Added code for performance figure
</commit_message>
<xml_diff>
--- a/data/default_rates_SP.xlsx
+++ b/data/default_rates_SP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumni-my.sharepoint.com/personal/qxb175_alumni_ku_dk/Documents/Dokumenter/10. semester/Seminar/CLOseminar/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C207B40-0CDE-425C-93E3-8311B48BBA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{6C207B40-0CDE-425C-93E3-8311B48BBA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E868A1B1-6D2F-4767-B9CA-033542AAA93D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{814FDA66-4DCA-4B8E-9E4F-060D7A7F0FFA}"/>
   </bookViews>
@@ -892,7 +892,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="P10" sqref="B10:P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated with adjusted probabilities
</commit_message>
<xml_diff>
--- a/data/default_rates_SP.xlsx
+++ b/data/default_rates_SP.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumni-my.sharepoint.com/personal/qxb175_alumni_ku_dk/Documents/Dokumenter/10. semester/Seminar/CLOseminar/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{6C207B40-0CDE-425C-93E3-8311B48BBA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E868A1B1-6D2F-4767-B9CA-033542AAA93D}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{6C207B40-0CDE-425C-93E3-8311B48BBA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7AD52F1-AD3F-49D2-B389-4CCD28A2B657}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{814FDA66-4DCA-4B8E-9E4F-060D7A7F0FFA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="adjust" sheetId="2" r:id="rId1"/>
+    <sheet name="no_adjust" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="157">
   <si>
     <t>Global Corporate Average Cumulative Default Rates (1981-2021)</t>
   </si>
@@ -563,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -573,6 +574,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -590,6 +594,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -888,11 +896,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F1B92B-689D-4FF2-AC45-16EA109580E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2679F3B2-A0AE-42BB-9C3A-3F632A9B109E}">
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="P10" sqref="B10:P10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -962,6 +970,597 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="5">
+        <f>0.306*B5</f>
+        <v>6.1200000000000004E-3</v>
+      </c>
+      <c r="C4" s="5">
+        <f t="shared" ref="C4:P4" si="0">0.306*C5</f>
+        <v>1.8359999999999998E-2</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="0"/>
+        <v>3.3660000000000002E-2</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
+        <v>6.1200000000000004E-2</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="0"/>
+        <v>9.1799999999999993E-2</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.12240000000000001</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.14687999999999998</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.16830000000000001</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.18972</v>
+      </c>
+      <c r="K4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.20808000000000001</v>
+      </c>
+      <c r="L4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.22644</v>
+      </c>
+      <c r="M4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.24480000000000002</v>
+      </c>
+      <c r="N4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.26316000000000001</v>
+      </c>
+      <c r="O4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.27845999999999999</v>
+      </c>
+      <c r="P4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.29375999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F1B92B-689D-4FF2-AC45-16EA109580E7}">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView zoomScale="93" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>6</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4">
+        <v>8</v>
+      </c>
+      <c r="J3" s="4">
+        <v>9</v>
+      </c>
+      <c r="K3" s="4">
+        <v>10</v>
+      </c>
+      <c r="L3" s="4">
+        <v>11</v>
+      </c>
+      <c r="M3" s="4">
+        <v>12</v>
+      </c>
+      <c r="N3" s="4">
+        <v>13</v>
+      </c>
+      <c r="O3" s="4">
+        <v>14</v>
+      </c>
+      <c r="P3" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added additional figures for result section
</commit_message>
<xml_diff>
--- a/data/default_rates_SP.xlsx
+++ b/data/default_rates_SP.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumni-my.sharepoint.com/personal/qxb175_alumni_ku_dk/Documents/Dokumenter/10. semester/Seminar/CLOseminar/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{6C207B40-0CDE-425C-93E3-8311B48BBA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7AD52F1-AD3F-49D2-B389-4CCD28A2B657}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{6C207B40-0CDE-425C-93E3-8311B48BBA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2922E12E-5813-4405-B39D-4BCA4CB67725}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{814FDA66-4DCA-4B8E-9E4F-060D7A7F0FFA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{814FDA66-4DCA-4B8E-9E4F-060D7A7F0FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="adjust" sheetId="2" r:id="rId1"/>
     <sheet name="no_adjust" sheetId="1" r:id="rId2"/>
+    <sheet name="master" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="157">
   <si>
     <t>Global Corporate Average Cumulative Default Rates (1981-2021)</t>
   </si>
@@ -514,7 +515,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,6 +544,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -561,10 +576,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -579,9 +595,19 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{58CB8119-F70B-4AC3-8427-DCAE31080C73}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -899,7 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2679F3B2-A0AE-42BB-9C3A-3F632A9B109E}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+    <sheetView zoomScale="93" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2060,4 +2086,400 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298C423B-29A7-44D5-834F-78D70F326044}">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>6</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4">
+        <v>8</v>
+      </c>
+      <c r="J3" s="4">
+        <v>9</v>
+      </c>
+      <c r="K3" s="4">
+        <v>10</v>
+      </c>
+      <c r="L3" s="4">
+        <v>11</v>
+      </c>
+      <c r="M3" s="4">
+        <v>12</v>
+      </c>
+      <c r="N3" s="4">
+        <v>13</v>
+      </c>
+      <c r="O3" s="4">
+        <v>14</v>
+      </c>
+      <c r="P3" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="D4" s="8">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.189</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.40599999999999997</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.45629629629629631</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.52499999999999991</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.11</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.41</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.49</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.63</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.13</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.22</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.46</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.76</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="J6" s="7">
+        <v>1.05</v>
+      </c>
+      <c r="K6" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.43</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1.54</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1.94</v>
+      </c>
+      <c r="H7" s="7">
+        <v>2.27</v>
+      </c>
+      <c r="I7" s="7">
+        <v>2.61</v>
+      </c>
+      <c r="J7" s="7">
+        <v>2.94</v>
+      </c>
+      <c r="K7" s="7">
+        <v>3.24</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.63</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1.93</v>
+      </c>
+      <c r="D8" s="7">
+        <v>3.46</v>
+      </c>
+      <c r="E8" s="7">
+        <v>4.99</v>
+      </c>
+      <c r="F8" s="7">
+        <v>6.43</v>
+      </c>
+      <c r="G8" s="7">
+        <v>7.75</v>
+      </c>
+      <c r="H8" s="7">
+        <v>8.89</v>
+      </c>
+      <c r="I8" s="7">
+        <v>9.9</v>
+      </c>
+      <c r="J8" s="7">
+        <v>10.82</v>
+      </c>
+      <c r="K8" s="7">
+        <v>11.64</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="7">
+        <v>3.34</v>
+      </c>
+      <c r="C9" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="D9" s="7">
+        <v>11.75</v>
+      </c>
+      <c r="E9" s="7">
+        <v>14.89</v>
+      </c>
+      <c r="F9" s="7">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="G9" s="7">
+        <v>19.36</v>
+      </c>
+      <c r="H9" s="7">
+        <v>20.99</v>
+      </c>
+      <c r="I9" s="7">
+        <v>22.31</v>
+      </c>
+      <c r="J9" s="7">
+        <v>23.5</v>
+      </c>
+      <c r="K9" s="7">
+        <v>24.62</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Various small changes, figures updated
</commit_message>
<xml_diff>
--- a/data/default_rates_SP.xlsx
+++ b/data/default_rates_SP.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="15" documentId="8_{6C207B40-0CDE-425C-93E3-8311B48BBA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2922E12E-5813-4405-B39D-4BCA4CB67725}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{814FDA66-4DCA-4B8E-9E4F-060D7A7F0FFA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{814FDA66-4DCA-4B8E-9E4F-060D7A7F0FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="adjust" sheetId="2" r:id="rId1"/>
@@ -925,9 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2679F3B2-A0AE-42BB-9C3A-3F632A9B109E}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView zoomScale="93" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2092,7 +2090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298C423B-29A7-44D5-834F-78D70F326044}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+    <sheetView zoomScale="93" workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>

</xml_diff>